<commit_message>
mouse figs for paper
</commit_message>
<xml_diff>
--- a/analysis/Mouse2/Human_Mouse Annotation.xlsx
+++ b/analysis/Mouse2/Human_Mouse Annotation.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-33060" yWindow="2920" windowWidth="25040" windowHeight="17000" tabRatio="500"/>
+    <workbookView xWindow="-33060" yWindow="2925" windowWidth="25035" windowHeight="16440" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="36">
   <si>
     <t>exon2</t>
   </si>
@@ -109,19 +105,44 @@
   </si>
   <si>
     <t>*cannot find a matching annotated exon</t>
+  </si>
+  <si>
+    <t>Exon</t>
+  </si>
+  <si>
+    <t>Stop</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>fullStop</t>
+  </si>
+  <si>
+    <t>fullStart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -151,16 +172,316 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -220,40 +541,238 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="45" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="47">
+    <cellStyle name="20% - Accent1" xfId="22" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="26" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="30" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="34" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="38" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="42" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="23" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="27" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="31" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="35" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="39" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="43" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="24" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="28" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="32" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="36" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="40" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="44" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="21" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="25" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="29" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="33" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="37" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="41" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="11" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="15" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="17" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="19" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="10" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="9" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Input" xfId="13" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="16" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="12" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="45"/>
+    <cellStyle name="Note 2" xfId="46"/>
+    <cellStyle name="Output" xfId="14" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="20" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="18" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -581,25 +1100,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:I1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="F1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="F1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
@@ -754,12 +1273,12 @@
       <c r="G7" s="1">
         <v>90704066</v>
       </c>
-      <c r="H7" s="1">
-        <v>90704372</v>
+      <c r="H7" s="4">
+        <v>90704367</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="0"/>
-        <v>306</v>
+        <f>H7-G7</f>
+        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1075,10 +1594,16 @@
       <c r="F19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="3" t="s">
+      <c r="G19" s="3">
+        <v>90561802</v>
+      </c>
+      <c r="H19" s="3">
+        <v>90561828</v>
+      </c>
+      <c r="I19" s="1">
+        <v>26</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1105,7 +1630,7 @@
         <v>90560860</v>
       </c>
       <c r="I20" s="1">
-        <f>H20-G20</f>
+        <f t="shared" ref="I20:I27" si="1">H20-G20</f>
         <v>119</v>
       </c>
     </row>
@@ -1132,7 +1657,7 @@
         <v>90362941</v>
       </c>
       <c r="I21" s="1">
-        <f>H21-G21</f>
+        <f t="shared" si="1"/>
         <v>181</v>
       </c>
     </row>
@@ -1159,7 +1684,7 @@
         <v>90208494</v>
       </c>
       <c r="I22" s="1">
-        <f>H22-G22</f>
+        <f t="shared" si="1"/>
         <v>171</v>
       </c>
     </row>
@@ -1186,7 +1711,7 @@
         <v>90163881</v>
       </c>
       <c r="I23" s="1">
-        <f>H23-G23</f>
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
     </row>
@@ -1213,7 +1738,7 @@
         <v>90162433</v>
       </c>
       <c r="I24" s="1">
-        <f>H24-G24</f>
+        <f t="shared" si="1"/>
         <v>319</v>
       </c>
     </row>
@@ -1240,7 +1765,7 @@
         <v>90059563</v>
       </c>
       <c r="I25" s="1">
-        <f>H25-G25</f>
+        <f t="shared" si="1"/>
         <v>78</v>
       </c>
     </row>
@@ -1267,7 +1792,7 @@
         <v>90059563</v>
       </c>
       <c r="I26" s="1">
-        <f>H26-G26</f>
+        <f t="shared" si="1"/>
         <v>87</v>
       </c>
     </row>
@@ -1294,7 +1819,7 @@
         <v>90037384</v>
       </c>
       <c r="I27" s="1">
-        <f>H27-G27</f>
+        <f t="shared" si="1"/>
         <v>484</v>
       </c>
     </row>
@@ -1324,11 +1849,587 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>91087955</v>
+      </c>
+      <c r="C2" s="1">
+        <v>91089605</v>
+      </c>
+      <c r="D2" s="1">
+        <f>F2-E2</f>
+        <v>1650</v>
+      </c>
+      <c r="E2" s="1">
+        <v>91087955</v>
+      </c>
+      <c r="F2" s="1">
+        <v>91089605</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>90995476</v>
+      </c>
+      <c r="C3" s="1">
+        <v>90995478</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D27" si="0">F3-E3</f>
+        <v>17</v>
+      </c>
+      <c r="E3" s="1">
+        <v>90995461</v>
+      </c>
+      <c r="F3" s="1">
+        <v>90995478</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>90995461</v>
+      </c>
+      <c r="C4" s="1">
+        <v>90995475</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E4" s="1">
+        <v>90995461</v>
+      </c>
+      <c r="F4" s="1">
+        <v>90995475</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>90992115</v>
+      </c>
+      <c r="C5" s="1">
+        <v>90992144</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="E5" s="1">
+        <v>90992115</v>
+      </c>
+      <c r="F5" s="1">
+        <v>90992144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>90991367</v>
+      </c>
+      <c r="C6" s="1">
+        <v>90991378</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E6" s="1">
+        <v>90991367</v>
+      </c>
+      <c r="F6" s="1">
+        <v>90991378</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>90704066</v>
+      </c>
+      <c r="C7" s="4">
+        <v>90704367</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>301</v>
+      </c>
+      <c r="E7" s="1">
+        <v>90704066</v>
+      </c>
+      <c r="F7" s="4">
+        <v>90704367</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>90701988</v>
+      </c>
+      <c r="C8" s="1">
+        <v>90702011</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E8" s="1">
+        <v>90701988</v>
+      </c>
+      <c r="F8" s="1">
+        <v>90702011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>90701967</v>
+      </c>
+      <c r="C9" s="1">
+        <v>90701987</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="E9" s="1">
+        <v>90701967</v>
+      </c>
+      <c r="F9" s="1">
+        <v>90702011</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>90700744</v>
+      </c>
+      <c r="C10" s="1">
+        <v>90700905</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>161</v>
+      </c>
+      <c r="E10" s="1">
+        <v>90700744</v>
+      </c>
+      <c r="F10" s="1">
+        <v>90700905</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>90642991</v>
+      </c>
+      <c r="C11" s="1">
+        <v>90643429</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>438</v>
+      </c>
+      <c r="E11" s="1">
+        <v>90642991</v>
+      </c>
+      <c r="F11" s="1">
+        <v>90643429</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>90629885</v>
+      </c>
+      <c r="C12" s="1">
+        <v>90630268</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>383</v>
+      </c>
+      <c r="E12" s="1">
+        <v>90629885</v>
+      </c>
+      <c r="F12" s="1">
+        <v>90630268</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>90623420</v>
+      </c>
+      <c r="C13" s="1">
+        <v>90623623</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>203</v>
+      </c>
+      <c r="E13" s="1">
+        <v>90623420</v>
+      </c>
+      <c r="F13" s="1">
+        <v>90623623</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>90620865</v>
+      </c>
+      <c r="C14" s="1">
+        <v>90620891</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="E14" s="1">
+        <v>90620865</v>
+      </c>
+      <c r="F14" s="1">
+        <v>90620891</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>90597507</v>
+      </c>
+      <c r="C15" s="1">
+        <v>90597629</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>122</v>
+      </c>
+      <c r="E15" s="1">
+        <v>90597507</v>
+      </c>
+      <c r="F15" s="1">
+        <v>90597629</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>90589848</v>
+      </c>
+      <c r="C16" s="1">
+        <v>90590229</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>381</v>
+      </c>
+      <c r="E16" s="1">
+        <v>90589848</v>
+      </c>
+      <c r="F16" s="1">
+        <v>90590229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>90588671</v>
+      </c>
+      <c r="C17" s="1">
+        <v>90588861</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>190</v>
+      </c>
+      <c r="E17" s="1">
+        <v>90588671</v>
+      </c>
+      <c r="F17" s="1">
+        <v>90588861</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>90565305</v>
+      </c>
+      <c r="C18" s="1">
+        <v>90565478</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>173</v>
+      </c>
+      <c r="E18" s="1">
+        <v>90565305</v>
+      </c>
+      <c r="F18" s="1">
+        <v>90565478</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3">
+        <v>90561802</v>
+      </c>
+      <c r="C19" s="3">
+        <v>90561828</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="E19" s="3">
+        <v>90561802</v>
+      </c>
+      <c r="F19" s="3">
+        <v>90561828</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>90560741</v>
+      </c>
+      <c r="C20" s="1">
+        <v>90560860</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="E20" s="1">
+        <v>90560741</v>
+      </c>
+      <c r="F20" s="1">
+        <v>90560860</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>90362760</v>
+      </c>
+      <c r="C21" s="1">
+        <v>90362941</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>181</v>
+      </c>
+      <c r="E21" s="1">
+        <v>90362760</v>
+      </c>
+      <c r="F21" s="1">
+        <v>90362941</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1">
+        <v>90208323</v>
+      </c>
+      <c r="C22" s="1">
+        <v>90208494</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>171</v>
+      </c>
+      <c r="E22" s="1">
+        <v>90208323</v>
+      </c>
+      <c r="F22" s="1">
+        <v>90208494</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1">
+        <v>90163792</v>
+      </c>
+      <c r="C23" s="1">
+        <v>90163881</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="E23" s="1">
+        <v>90163792</v>
+      </c>
+      <c r="F23" s="1">
+        <v>90163881</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1">
+        <v>90162114</v>
+      </c>
+      <c r="C24" s="1">
+        <v>90162433</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>319</v>
+      </c>
+      <c r="E24" s="1">
+        <v>90162114</v>
+      </c>
+      <c r="F24" s="1">
+        <v>90162433</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>90059485</v>
+      </c>
+      <c r="C25" s="1">
+        <v>90059563</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="E25" s="1">
+        <v>90059485</v>
+      </c>
+      <c r="F25" s="1">
+        <v>90059563</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1">
+        <v>90059476</v>
+      </c>
+      <c r="C26" s="1">
+        <v>90059484</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="E26" s="1">
+        <v>90059476</v>
+      </c>
+      <c r="F26" s="1">
+        <v>90059563</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1">
+        <v>90036900</v>
+      </c>
+      <c r="C27" s="1">
+        <v>90037384</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>484</v>
+      </c>
+      <c r="E27" s="1">
+        <v>90036900</v>
+      </c>
+      <c r="F27" s="1">
+        <v>90037384</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>